<commit_message>
Altered raw data to include categorical variable
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC7C0DA1-2246-E849-8A1E-81208D236FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D7610D-5E34-1444-AFAB-ED0DE3A2B25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45600" yWindow="6380" windowWidth="19020" windowHeight="12320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18660" yWindow="10560" windowWidth="19020" windowHeight="12320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -74,52 +74,34 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
-    <t>First Letter of Cat's Name</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>Cat Age</t>
   </si>
   <si>
     <t xml:space="preserve">Cat Age </t>
   </si>
   <si>
-    <t>letters from Roman alphabet</t>
-  </si>
-  <si>
     <t>age in years</t>
   </si>
   <si>
-    <t>roman alphabet characters  (A:Z) or NA</t>
+    <t>Cat Breed</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Breed of the individual's cat (Siamese /Maine Coon/American Shorthair/Persian)</t>
+  </si>
+  <si>
+    <t>S/MC/AS/P/NA</t>
   </si>
 </sst>
 </file>
@@ -448,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,10 +447,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -482,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -499,7 +481,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>7</v>
@@ -516,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -533,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -550,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -567,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -584,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -601,7 +583,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -635,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -649,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -666,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>17</v>
@@ -700,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -716,7 +698,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -772,21 +754,21 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>

</xml_diff>